<commit_message>
Auto-committed on 2022/01/04 週二
Former-commit-id: 43271d1aece305d2522154852e935c77ec51c504
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/EmpDeductMedia.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/EmpDeductMedia.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -185,10 +185,6 @@
   <si>
     <t>EmpDeductMedia</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ErrorCode</t>
-    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>CustId</t>
@@ -527,41 +523,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">16: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>扣款失敗</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">17: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>扣款不足</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>OccUnknowC</t>
   </si>
   <si>
@@ -601,9 +562,6 @@
   <si>
     <t>OccAcctAmt</t>
     <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>實扣金額</t>
   </si>
   <si>
     <t>OccEntryDate</t>
@@ -728,10 +686,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>01:扣款成功 16:扣款失敗 17:扣款不足…..</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>有回應檔均會更新</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -757,6 +711,28 @@
   <si>
     <t>EntryDate &gt;= , AND EntryDate &lt;= , AND MediaKind =</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>實扣金額</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrorCode</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>回應檔失敗原因參考 : 
+ref. CdCode ProcCode 處理說明
+員工扣薪 : 004 + ReturnCode(2)
+01:扣款成功
+16:扣款失敗 (扣款金額=0)
+17:扣款不足 (扣款金額 !=0 且 扣款金額＜應扣金額)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 扣款失敗 (扣款金額=0)
+17 扣款不足 (扣款金額 !=0 且 扣款金額＜應扣金額)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1380,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -1414,7 +1390,7 @@
       <c r="A2" s="32"/>
       <c r="B2" s="33"/>
       <c r="C2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>3</v>
@@ -1429,7 +1405,7 @@
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>17</v>
@@ -1468,7 +1444,7 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="10"/>
@@ -1481,7 +1457,7 @@
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="10"/>
@@ -1516,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>32</v>
@@ -1535,10 +1511,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>29</v>
@@ -1548,7 +1524,7 @@
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="15" customFormat="1">
@@ -1556,7 +1532,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>33</v>
@@ -1575,10 +1551,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>28</v>
@@ -1593,10 +1569,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>28</v>
@@ -1605,7 +1581,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="32.4">
@@ -1613,10 +1589,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>28</v>
@@ -1625,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1651,7 +1627,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>24</v>
@@ -1669,7 +1645,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>36</v>
@@ -1690,7 +1666,7 @@
         <v>39</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>29</v>
@@ -1705,7 +1681,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>25</v>
@@ -1726,7 +1702,7 @@
         <v>43</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>38</v>
@@ -1754,12 +1730,12 @@
       </c>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="97.2">
       <c r="A22" s="19">
         <v>14</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>26</v>
@@ -1770,8 +1746,8 @@
       <c r="E22" s="19">
         <v>2</v>
       </c>
-      <c r="G22" s="24" t="s">
-        <v>147</v>
+      <c r="G22" s="31" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1791,7 +1767,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1799,7 +1775,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>21</v>
@@ -1811,7 +1787,7 @@
         <v>8</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1819,7 +1795,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>22</v>
@@ -1855,13 +1831,13 @@
         <v>19</v>
       </c>
       <c r="B27" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="D27" s="25" t="s">
         <v>53</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>54</v>
       </c>
       <c r="E27" s="23"/>
       <c r="G27" s="24"/>
@@ -1871,13 +1847,13 @@
         <v>20</v>
       </c>
       <c r="B28" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="D28" s="25" t="s">
         <v>56</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>57</v>
       </c>
       <c r="E28" s="23">
         <v>6</v>
@@ -1889,13 +1865,13 @@
         <v>21</v>
       </c>
       <c r="B29" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="D29" s="25" t="s">
         <v>59</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>60</v>
       </c>
       <c r="E29" s="23"/>
       <c r="G29" s="24"/>
@@ -1905,13 +1881,13 @@
         <v>22</v>
       </c>
       <c r="B30" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>62</v>
-      </c>
       <c r="D30" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="23">
         <v>6</v>
@@ -1938,7 +1914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
@@ -1972,57 +1948,57 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2037,7 +2013,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -2057,12 +2033,12 @@
     <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27" customWidth="1"/>
+    <col min="17" max="17" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -2072,7 +2048,7 @@
       <c r="G1" s="36"/>
       <c r="H1" s="36"/>
       <c r="J1" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K1" s="36"/>
       <c r="L1" s="36"/>
@@ -2084,52 +2060,52 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="G2" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="H2" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>87</v>
-      </c>
       <c r="J2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="L2" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="M2" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="N2" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="O2" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="P2" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="Q2" s="26" t="s">
         <v>86</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2137,13 +2113,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="26">
         <v>7</v>
@@ -2155,19 +2131,19 @@
         <v>7</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J3" s="26">
         <v>1</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L3" s="27" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N3" s="26">
         <v>7</v>
@@ -2179,7 +2155,7 @@
         <v>7</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2187,13 +2163,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>92</v>
-      </c>
       <c r="D4" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="26">
         <v>6</v>
@@ -2207,19 +2183,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J4" s="26">
         <v>2</v>
       </c>
       <c r="K4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="27" t="s">
-        <v>92</v>
-      </c>
       <c r="M4" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N4" s="26">
         <v>6</v>
@@ -2233,7 +2209,7 @@
         <v>13</v>
       </c>
       <c r="Q4" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="32.4">
@@ -2241,13 +2217,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="D5" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="E5" s="26">
         <v>10</v>
@@ -2261,19 +2237,19 @@
         <v>23</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J5" s="26">
         <v>3</v>
       </c>
       <c r="K5" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="L5" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="M5" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M5" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="N5" s="26">
         <v>10</v>
@@ -2287,7 +2263,7 @@
         <v>23</v>
       </c>
       <c r="Q5" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2297,13 +2273,13 @@
         <v>4</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L6" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M6" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="N6" s="26">
         <v>2</v>
@@ -2317,7 +2293,7 @@
         <v>25</v>
       </c>
       <c r="Q6" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2325,13 +2301,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="26">
         <v>10</v>
@@ -2349,13 +2325,13 @@
         <v>5</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L7" s="27" t="s">
         <v>25</v>
       </c>
       <c r="M7" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N7" s="26">
         <v>10</v>
@@ -2370,18 +2346,18 @@
       </c>
       <c r="Q7" s="27"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" ht="46.8">
       <c r="A8" s="26">
         <v>5</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="26">
         <v>11</v>
@@ -2395,19 +2371,19 @@
         <v>44</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J8" s="26">
         <v>6</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L8" s="27" t="s">
         <v>26</v>
       </c>
       <c r="M8" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N8" s="26">
         <v>2</v>
@@ -2421,7 +2397,7 @@
         <v>37</v>
       </c>
       <c r="Q8" s="27" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2429,13 +2405,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="26">
         <v>11</v>
@@ -2449,19 +2425,19 @@
         <v>55</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J9" s="26">
         <v>7</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L9" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N9" s="26">
         <v>7</v>
@@ -2475,7 +2451,7 @@
         <v>44</v>
       </c>
       <c r="Q9" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2485,13 +2461,13 @@
         <v>8</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M10" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N10" s="26">
         <v>15</v>
@@ -2511,13 +2487,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" s="26">
         <v>10</v>
@@ -2537,13 +2513,13 @@
         <v>9</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M11" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N11" s="26">
         <v>10</v>
@@ -2565,13 +2541,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="26">
         <v>40</v>
@@ -2585,19 +2561,19 @@
         <v>105</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J12" s="26">
         <v>10</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M12" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N12" s="26">
         <v>40</v>
@@ -2617,13 +2593,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" s="26">
         <v>1</v>
@@ -2637,19 +2613,19 @@
         <v>106</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J13" s="26">
         <v>11</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L13" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M13" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N13" s="26">
         <v>1</v>
@@ -2663,7 +2639,7 @@
         <v>110</v>
       </c>
       <c r="Q13" s="27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2673,13 +2649,13 @@
         <v>12</v>
       </c>
       <c r="K14" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="27" t="s">
-        <v>96</v>
-      </c>
       <c r="M14" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N14" s="26">
         <v>14</v>
@@ -2693,7 +2669,7 @@
         <v>124</v>
       </c>
       <c r="Q14" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2703,13 +2679,13 @@
         <v>13</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L15" s="27" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="M15" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N15" s="26">
         <v>10</v>
@@ -2731,13 +2707,13 @@
         <v>10</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E16" s="26">
         <v>8</v>
@@ -2751,19 +2727,19 @@
         <v>114</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J16" s="26">
         <v>14</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L16" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M16" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N16" s="26">
         <v>8</v>
@@ -2777,7 +2753,7 @@
         <v>142</v>
       </c>
       <c r="Q16" s="27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2785,13 +2761,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E17" s="26">
         <v>6</v>
@@ -2805,19 +2781,19 @@
         <v>120</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J17" s="26">
         <v>15</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L17" s="27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="M17" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N17" s="26">
         <v>6</v>
@@ -2831,7 +2807,7 @@
         <v>148</v>
       </c>
       <c r="Q17" s="27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2839,13 +2815,13 @@
         <v>12</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" s="26">
         <v>1</v>
@@ -2863,13 +2839,13 @@
         <v>16</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L18" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M18" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N18" s="26">
         <v>1</v>
@@ -2889,13 +2865,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E19" s="26">
         <v>1</v>
@@ -2913,13 +2889,13 @@
         <v>17</v>
       </c>
       <c r="K19" s="26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L19" s="27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M19" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N19" s="26">
         <v>1</v>
@@ -2939,13 +2915,13 @@
         <v>14</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E20" s="26">
         <v>7</v>
@@ -2963,13 +2939,13 @@
         <v>18</v>
       </c>
       <c r="K20" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L20" s="27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="M20" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N20" s="26">
         <v>7</v>
@@ -2989,13 +2965,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E21" s="26">
         <v>3</v>
@@ -3013,13 +2989,13 @@
         <v>19</v>
       </c>
       <c r="K21" s="26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L21" s="27" t="s">
         <v>27</v>
       </c>
       <c r="M21" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N21" s="26">
         <v>3</v>
@@ -3039,13 +3015,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E22" s="26">
         <v>42</v>
@@ -3059,19 +3035,19 @@
         <v>174</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J22" s="26">
         <v>20</v>
       </c>
       <c r="K22" s="26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L22" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M22" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N22" s="26">
         <v>42</v>

</xml_diff>

<commit_message>
Auto-committed on 2022/01/06 週四
Former-commit-id: c46be7755217e3576507cbf02a733689f46283a4
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/EmpDeductMedia.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/EmpDeductMedia.xlsx
@@ -721,18 +721,18 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
+    <t>16 扣款失敗 (扣款金額=0)
+17 扣款不足 (扣款金額 !=0 且 扣款金額＜應扣金額)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
     <t>回應檔失敗原因參考 : 
 ref. CdCode ProcCode 處理說明
 員工扣薪 : 004 + ReturnCode(2)
-01:扣款成功
+01:成功
 16:扣款失敗 (扣款金額=0)
 17:扣款不足 (扣款金額 !=0 且 扣款金額＜應扣金額)</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>16 扣款失敗 (扣款金額=0)
-17 扣款不足 (扣款金額 !=0 且 扣款金額＜應扣金額)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1357,7 +1357,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -1747,7 +1747,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2397,7 +2397,7 @@
         <v>37</v>
       </c>
       <c r="Q8" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:17">

</xml_diff>